<commit_message>
compute frequency lr IM
</commit_message>
<xml_diff>
--- a/LO6/IM/data.xlsx
+++ b/LO6/IM/data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erwinplanck/Desktop/Physics/Physics Lab III/LO6/IM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23357F7E-4EE4-5843-B0EB-4E18DB82974C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DBDEA9-2E60-3D46-BBD5-347494C82487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="28720" windowHeight="15940" xr2:uid="{BE3B2C25-128F-C64E-BA69-1E61889D2033}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>mario guapo y ceballos</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>We are assuming that distro is gaussian even though its not</t>
+  </si>
+  <si>
+    <t>m</t>
   </si>
 </sst>
 </file>
@@ -478,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2944EC20-B223-6B47-A13A-DE0E5E7D6228}">
   <dimension ref="B2:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,7 +623,49 @@
         <v>585532.1</v>
       </c>
     </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+      <c r="K15">
+        <v>5</v>
+      </c>
+      <c r="L15">
+        <v>6</v>
+      </c>
+      <c r="M15">
+        <v>7</v>
+      </c>
+      <c r="N15">
+        <v>8</v>
+      </c>
+      <c r="O15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <f>11.3/3</f>
+        <v>3.7666666666666671</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <f>14.9/4</f>
+        <v>3.7250000000000001</v>
+      </c>
       <c r="F20">
         <v>170</v>
       </c>
@@ -629,13 +674,13 @@
         <v>111.00000000000011</v>
       </c>
     </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="G21">
         <f>(13.42-F12)*100</f>
         <v>113.00000000000009</v>
       </c>
     </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="G22" t="s">
         <v>17</v>
       </c>
@@ -647,12 +692,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="F25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="E26">
         <v>12.34</v>
       </c>
@@ -661,7 +706,7 @@
         <v>0.10000000000000142</v>
       </c>
     </row>
-    <row r="27" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="E27">
         <v>12.35</v>
       </c>
@@ -670,12 +715,12 @@
         <v>0.12000000000000099</v>
       </c>
     </row>
-    <row r="29" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
       <c r="F29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
       <c r="E30">
         <v>1</v>
       </c>
@@ -693,7 +738,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
       <c r="G31">
         <v>476617.6</v>
       </c>
@@ -701,7 +746,7 @@
         <v>468425.7</v>
       </c>
     </row>
-    <row r="32" spans="5:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
       <c r="F32" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Upload figs on IM
</commit_message>
<xml_diff>
--- a/LO6/IM/data.xlsx
+++ b/LO6/IM/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erwinplanck/Desktop/Physics/Physics Lab III/LO6/IM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86734F93-CD1F-034C-9B83-C2193C8D11A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F0EE2E-B3E1-1843-95B8-F08CE1C141D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="28720" windowHeight="15940" xr2:uid="{BE3B2C25-128F-C64E-BA69-1E61889D2033}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>mario guapo y ceballos</t>
   </si>
@@ -145,13 +145,16 @@
   </si>
   <si>
     <t>t</t>
+  </si>
+  <si>
+    <t>DISCARDED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -162,6 +165,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -199,11 +209,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,7 +537,7 @@
   <dimension ref="B2:U38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -769,7 +780,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="5:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:21" x14ac:dyDescent="0.2">
       <c r="Q17">
         <v>42325362626.521507</v>
       </c>
@@ -783,12 +794,12 @@
         <v>21811239.11538909</v>
       </c>
     </row>
-    <row r="19" spans="5:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="5:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F20">
         <v>170</v>
       </c>
@@ -805,7 +816,7 @@
         <v>5.647633951993983E-6</v>
       </c>
     </row>
-    <row r="21" spans="5:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:21" x14ac:dyDescent="0.2">
       <c r="G21">
         <f>(13.42-F12)*100</f>
         <v>113.00000000000009</v>
@@ -819,7 +830,7 @@
         <v>7.4443725465105817E-6</v>
       </c>
     </row>
-    <row r="22" spans="5:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:21" x14ac:dyDescent="0.2">
       <c r="G22" t="s">
         <v>17</v>
       </c>
@@ -831,20 +842,20 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="5:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:21" x14ac:dyDescent="0.2">
       <c r="H23">
         <f>G21/F20</f>
         <v>0.6647058823529417</v>
       </c>
     </row>
-    <row r="25" spans="5:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="5:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="4:21" x14ac:dyDescent="0.2">
       <c r="E26">
-        <v>12.34</v>
+        <v>12.38</v>
       </c>
       <c r="F26">
         <v>10</v>
@@ -858,9 +869,9 @@
         <v>30000000000000.004</v>
       </c>
     </row>
-    <row r="27" spans="5:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="4:21" x14ac:dyDescent="0.2">
       <c r="E27">
-        <v>12.35</v>
+        <v>12.39</v>
       </c>
       <c r="F27">
         <v>12</v>
@@ -874,45 +885,52 @@
         <v>25000000000000</v>
       </c>
     </row>
-    <row r="29" spans="5:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="5:21" x14ac:dyDescent="0.2">
-      <c r="E30">
+    <row r="30" spans="4:21" x14ac:dyDescent="0.2">
+      <c r="D30" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="4">
         <v>1</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="4">
         <v>1576.08</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="4">
         <f>G30/2</f>
         <v>788.04</v>
       </c>
-      <c r="J30" t="s">
+      <c r="J30" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="5:21" x14ac:dyDescent="0.2">
-      <c r="G31">
+    <row r="31" spans="4:21" x14ac:dyDescent="0.2">
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4">
         <v>476617.6</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="4">
         <v>468425.7</v>
       </c>
     </row>
-    <row r="32" spans="5:21" x14ac:dyDescent="0.2">
-      <c r="F32" t="s">
+    <row r="32" spans="4:21" x14ac:dyDescent="0.2">
+      <c r="E32" s="4"/>
+      <c r="F32" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="4">
         <f>G31-H31</f>
         <v>8191.8999999999651</v>
       </c>
+      <c r="H32" s="4"/>
     </row>
     <row r="33" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E33">

</xml_diff>